<commit_message>
changed the aesthetics of the plot removed the grey background and relabeled axes. Lost the lm()
</commit_message>
<xml_diff>
--- a/samp_data-prototypeT.xlsx
+++ b/samp_data-prototypeT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/17e227d69cbbef2f/Desktop/KBH_2_Pyx_Therm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{3546B046-AFE3-4B87-92BE-772B5242DA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67DBA6CC-408E-4459-BDD0-26935CADD6B0}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{3546B046-AFE3-4B87-92BE-772B5242DA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{910D2975-E9E4-4C85-8057-2AA6CBE9DC54}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>rim</t>
   </si>
@@ -92,6 +92,102 @@
   </si>
   <si>
     <t>Nb_ions_Na_OPX</t>
+  </si>
+  <si>
+    <t>point_number_CPX</t>
+  </si>
+  <si>
+    <t>point_number_OPX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 1 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 2 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 3 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 4 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 5 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 6 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 7 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 8 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 9 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 10 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 11 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 12 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 13 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 14 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 / 15 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 1 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 2 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 3 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 4 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 5 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 6 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 7 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 8 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 9 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 10 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 11 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 12 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 13 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 14 . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 / 15 . </t>
   </si>
 </sst>
 </file>
@@ -941,828 +1037,926 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
-    <col min="3" max="8" width="9.140625" style="1"/>
-    <col min="9" max="11" width="17.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="19.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="5" max="10" width="9.140625" style="1"/>
+    <col min="11" max="13" width="17.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="E2" s="1">
         <v>-5190</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F2" s="1">
         <v>-5855</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G2" s="1">
         <v>-27104</v>
       </c>
-      <c r="F2" s="1">
+      <c r="H2" s="1">
         <v>-24690</v>
       </c>
-      <c r="G2" s="1">
+      <c r="I2" s="1">
         <v>139</v>
       </c>
-      <c r="H2" s="1">
+      <c r="J2" s="1">
         <v>150</v>
       </c>
-      <c r="I2" s="1">
+      <c r="K2" s="1">
         <v>0.84599999999999997</v>
       </c>
-      <c r="J2" s="1">
+      <c r="L2" s="1">
         <v>1.6379999999999999</v>
       </c>
-      <c r="K2" s="1">
+      <c r="M2" s="1">
         <v>0.128</v>
       </c>
-      <c r="L2" s="1">
+      <c r="N2" s="1">
         <v>0.222</v>
       </c>
-      <c r="M2" s="3">
+      <c r="O2" s="3">
         <v>0.74299999999999999</v>
       </c>
-      <c r="N2" s="2">
+      <c r="P2" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="O2" s="2">
+      <c r="Q2" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="P2" s="2">
+      <c r="R2" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="E3" s="1">
         <v>-4530</v>
       </c>
-      <c r="D3" s="1">
+      <c r="F3" s="1">
         <v>-5032</v>
       </c>
-      <c r="E3" s="1">
+      <c r="G3" s="1">
         <v>-27162</v>
       </c>
-      <c r="F3" s="1">
+      <c r="H3" s="1">
         <v>-25438</v>
       </c>
-      <c r="G3" s="1">
+      <c r="I3" s="1">
         <v>139</v>
       </c>
-      <c r="H3" s="1">
+      <c r="J3" s="1">
         <v>146</v>
       </c>
-      <c r="I3" s="1">
+      <c r="K3" s="1">
         <v>0.84399999999999997</v>
       </c>
-      <c r="J3" s="1">
+      <c r="L3" s="1">
         <v>1.62</v>
       </c>
-      <c r="K3" s="1">
+      <c r="M3" s="1">
         <v>0.127</v>
       </c>
-      <c r="L3" s="1">
+      <c r="N3" s="1">
         <v>0.22600000000000001</v>
       </c>
-      <c r="M3" s="3">
+      <c r="O3" s="3">
         <v>0.74099999999999999</v>
       </c>
-      <c r="N3" s="2">
+      <c r="P3" s="2">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="O3" s="2">
+      <c r="Q3" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="P3" s="2">
+      <c r="R3" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="E4" s="1">
         <v>1160</v>
       </c>
-      <c r="D4" s="1">
+      <c r="F4" s="1">
         <v>-3176</v>
       </c>
-      <c r="E4" s="1">
+      <c r="G4" s="1">
         <v>-29155</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <v>-27901</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
         <v>129</v>
       </c>
-      <c r="H4" s="1">
+      <c r="J4" s="1">
         <v>138</v>
       </c>
-      <c r="I4" s="1">
+      <c r="K4" s="1">
         <v>0.84499999999999997</v>
       </c>
-      <c r="J4" s="1">
+      <c r="L4" s="1">
         <v>1.6359999999999999</v>
       </c>
-      <c r="K4" s="1">
+      <c r="M4" s="1">
         <v>0.127</v>
       </c>
-      <c r="L4" s="1">
+      <c r="N4" s="1">
         <v>0.22500000000000001</v>
       </c>
-      <c r="M4" s="3">
+      <c r="O4" s="3">
         <v>0.73699999999999999</v>
       </c>
-      <c r="N4" s="2">
+      <c r="P4" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="O4" s="2">
+      <c r="Q4" s="2">
         <v>0.10100000000000001</v>
       </c>
-      <c r="P4" s="2">
+      <c r="R4" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="E5" s="1">
         <v>1247</v>
       </c>
-      <c r="D5" s="1">
+      <c r="F5" s="1">
         <v>162</v>
       </c>
-      <c r="E5" s="1">
+      <c r="G5" s="1">
         <v>-30822</v>
       </c>
-      <c r="F5" s="1">
+      <c r="H5" s="1">
         <v>-28862</v>
       </c>
-      <c r="G5" s="1">
+      <c r="I5" s="1">
         <v>128</v>
       </c>
-      <c r="H5" s="1">
+      <c r="J5" s="1">
         <v>135</v>
       </c>
-      <c r="I5" s="1">
+      <c r="K5" s="1">
         <v>0.84</v>
       </c>
-      <c r="J5" s="1">
+      <c r="L5" s="1">
         <v>1.623</v>
       </c>
-      <c r="K5" s="1">
+      <c r="M5" s="1">
         <v>0.13600000000000001</v>
       </c>
-      <c r="L5" s="1">
+      <c r="N5" s="1">
         <v>0.23100000000000001</v>
       </c>
-      <c r="M5" s="3">
+      <c r="O5" s="3">
         <v>0.746</v>
       </c>
-      <c r="N5" s="2">
+      <c r="P5" s="2">
         <v>3.9E-2</v>
       </c>
-      <c r="O5" s="2">
+      <c r="Q5" s="2">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="P5" s="2">
+      <c r="R5" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="E6" s="1">
         <v>-226</v>
       </c>
-      <c r="D6" s="1">
+      <c r="F6" s="1">
         <v>2688</v>
       </c>
-      <c r="E6" s="1">
+      <c r="G6" s="1">
         <v>-31114</v>
       </c>
-      <c r="F6" s="1">
+      <c r="H6" s="1">
         <v>-29738</v>
       </c>
-      <c r="G6" s="1">
+      <c r="I6" s="1">
         <v>124</v>
       </c>
-      <c r="H6" s="1">
+      <c r="J6" s="1">
         <v>127</v>
       </c>
-      <c r="I6" s="1">
+      <c r="K6" s="1">
         <v>0.84499999999999997</v>
       </c>
-      <c r="J6" s="1">
+      <c r="L6" s="1">
         <v>1.5960000000000001</v>
       </c>
-      <c r="K6" s="1">
+      <c r="M6" s="1">
         <v>0.13500000000000001</v>
       </c>
-      <c r="L6" s="1">
+      <c r="N6" s="1">
         <v>0.249</v>
       </c>
-      <c r="M6" s="3">
+      <c r="O6" s="3">
         <v>0.74</v>
       </c>
-      <c r="N6" s="2">
+      <c r="P6" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="O6" s="2">
+      <c r="Q6" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="P6" s="2">
+      <c r="R6" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
+      <c r="E7" s="1">
         <v>4855</v>
       </c>
-      <c r="D7" s="1">
+      <c r="F7" s="1">
         <v>3403</v>
       </c>
-      <c r="E7" s="1">
+      <c r="G7" s="1">
         <v>-31987</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H7" s="1">
         <v>-26027</v>
       </c>
-      <c r="G7" s="1">
+      <c r="I7" s="1">
         <v>117</v>
       </c>
-      <c r="H7" s="1">
+      <c r="J7" s="1">
         <v>140</v>
       </c>
-      <c r="I7" s="1">
+      <c r="K7" s="1">
         <v>0.83</v>
       </c>
-      <c r="J7" s="1">
+      <c r="L7" s="1">
         <v>1.593</v>
       </c>
-      <c r="K7" s="1">
+      <c r="M7" s="1">
         <v>0.14199999999999999</v>
       </c>
-      <c r="L7" s="1">
+      <c r="N7" s="1">
         <v>0.249</v>
       </c>
-      <c r="M7" s="3">
+      <c r="O7" s="3">
         <v>0.74</v>
       </c>
-      <c r="N7" s="2">
+      <c r="P7" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="O7" s="2">
+      <c r="Q7" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="P7" s="2">
+      <c r="R7" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1">
+      <c r="E8" s="1">
         <v>6610</v>
       </c>
-      <c r="D8" s="1">
+      <c r="F8" s="1">
         <v>11338</v>
       </c>
-      <c r="E8" s="1">
+      <c r="G8" s="1">
         <v>-32138</v>
       </c>
-      <c r="F8" s="1">
+      <c r="H8" s="1">
         <v>-28588</v>
       </c>
-      <c r="G8" s="1">
+      <c r="I8" s="1">
         <v>117</v>
       </c>
-      <c r="H8" s="1">
+      <c r="J8" s="1">
         <v>120</v>
       </c>
-      <c r="I8" s="1">
+      <c r="K8" s="1">
         <v>0.81200000000000006</v>
       </c>
-      <c r="J8" s="1">
+      <c r="L8" s="1">
         <v>1.5860000000000001</v>
       </c>
-      <c r="K8" s="1">
+      <c r="M8" s="1">
         <v>0.14799999999999999</v>
       </c>
-      <c r="L8" s="1">
+      <c r="N8" s="1">
         <v>0.25700000000000001</v>
       </c>
-      <c r="M8" s="3">
+      <c r="O8" s="3">
         <v>0.751</v>
       </c>
-      <c r="N8" s="2">
+      <c r="P8" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="O8" s="2">
+      <c r="Q8" s="2">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="P8" s="2">
+      <c r="R8" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1">
+      <c r="E9" s="1">
         <v>5642</v>
       </c>
-      <c r="D9" s="1">
+      <c r="F9" s="1">
         <v>12212</v>
       </c>
-      <c r="E9" s="1">
+      <c r="G9" s="1">
         <v>-31195</v>
       </c>
-      <c r="F9" s="1">
+      <c r="H9" s="1">
         <v>-27364</v>
       </c>
-      <c r="G9" s="1">
+      <c r="I9" s="1">
         <v>123</v>
       </c>
-      <c r="H9" s="1">
+      <c r="J9" s="1">
         <v>124</v>
       </c>
-      <c r="I9" s="1">
+      <c r="K9" s="1">
         <v>0.82199999999999995</v>
       </c>
-      <c r="J9" s="1">
+      <c r="L9" s="1">
         <v>1.5920000000000001</v>
       </c>
-      <c r="K9" s="1">
+      <c r="M9" s="1">
         <v>0.14199999999999999</v>
       </c>
-      <c r="L9" s="1">
+      <c r="N9" s="1">
         <v>0.25800000000000001</v>
       </c>
-      <c r="M9" s="3">
+      <c r="O9" s="3">
         <v>0.748</v>
       </c>
-      <c r="N9" s="2">
+      <c r="P9" s="2">
         <v>3.9E-2</v>
       </c>
-      <c r="O9" s="2">
+      <c r="Q9" s="2">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="P9" s="2">
+      <c r="R9" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="1">
+      <c r="E10" s="1">
         <v>5332</v>
       </c>
-      <c r="D10" s="1">
+      <c r="F10" s="1">
         <v>12355</v>
       </c>
-      <c r="E10" s="1">
+      <c r="G10" s="1">
         <v>-31292</v>
       </c>
-      <c r="F10" s="1">
+      <c r="H10" s="1">
         <v>-24835</v>
       </c>
-      <c r="G10" s="1">
+      <c r="I10" s="1">
         <v>123</v>
       </c>
-      <c r="H10" s="1">
+      <c r="J10" s="1">
         <v>133</v>
       </c>
-      <c r="I10" s="1">
+      <c r="K10" s="1">
         <v>0.84399999999999997</v>
       </c>
-      <c r="J10" s="1">
+      <c r="L10" s="1">
         <v>1.6</v>
       </c>
-      <c r="K10" s="1">
+      <c r="M10" s="1">
         <v>0.13700000000000001</v>
       </c>
-      <c r="L10" s="1">
+      <c r="N10" s="1">
         <v>0.255</v>
       </c>
-      <c r="M10" s="3">
+      <c r="O10" s="3">
         <v>0.82099999999999995</v>
       </c>
-      <c r="N10" s="2">
+      <c r="P10" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="O10" s="2">
+      <c r="Q10" s="2">
         <v>4.7E-2</v>
       </c>
-      <c r="P10" s="2">
+      <c r="R10" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
+      <c r="E11" s="1">
         <v>8553</v>
       </c>
-      <c r="D11" s="1">
+      <c r="F11" s="1">
         <v>13901</v>
       </c>
-      <c r="E11" s="1">
+      <c r="G11" s="1">
         <v>-33012</v>
       </c>
-      <c r="F11" s="1">
+      <c r="H11" s="1">
         <v>-24749</v>
       </c>
-      <c r="G11" s="1">
+      <c r="I11" s="1">
         <v>108</v>
       </c>
-      <c r="H11" s="1">
+      <c r="J11" s="1">
         <v>124</v>
       </c>
-      <c r="I11" s="1">
+      <c r="K11" s="1">
         <v>0.78900000000000003</v>
       </c>
-      <c r="J11" s="1">
+      <c r="L11" s="1">
         <v>1.601</v>
       </c>
-      <c r="K11" s="1">
+      <c r="M11" s="1">
         <v>0.151</v>
       </c>
-      <c r="L11" s="1">
+      <c r="N11" s="1">
         <v>0.24399999999999999</v>
       </c>
-      <c r="M11" s="3">
+      <c r="O11" s="3">
         <v>0.752</v>
       </c>
-      <c r="N11" s="2">
+      <c r="P11" s="2">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="O11" s="2">
+      <c r="Q11" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="P11" s="2">
+      <c r="R11" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
+      <c r="E12" s="1">
         <v>8960</v>
       </c>
-      <c r="D12" s="1">
+      <c r="F12" s="1">
         <v>17511</v>
       </c>
-      <c r="E12" s="1">
+      <c r="G12" s="1">
         <v>-32963</v>
       </c>
-      <c r="F12" s="1">
+      <c r="H12" s="1">
         <v>-25622</v>
       </c>
-      <c r="G12" s="1">
+      <c r="I12" s="1">
         <v>108</v>
       </c>
-      <c r="H12" s="1">
+      <c r="J12" s="1">
         <v>116</v>
       </c>
-      <c r="I12" s="1">
+      <c r="K12" s="1">
         <v>0.88700000000000001</v>
       </c>
-      <c r="J12" s="1">
+      <c r="L12" s="1">
         <v>1.5880000000000001</v>
       </c>
-      <c r="K12" s="1">
+      <c r="M12" s="1">
         <v>0.108</v>
       </c>
-      <c r="L12" s="1">
+      <c r="N12" s="1">
         <v>0.26400000000000001</v>
       </c>
-      <c r="M12" s="3">
+      <c r="O12" s="3">
         <v>0.83</v>
       </c>
-      <c r="N12" s="2">
+      <c r="P12" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="O12" s="2">
+      <c r="Q12" s="2">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="P12" s="2">
+      <c r="R12" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="1">
+      <c r="E13" s="1">
         <v>9599</v>
       </c>
-      <c r="D13" s="1">
+      <c r="F13" s="1">
         <v>18357</v>
       </c>
-      <c r="E13" s="1">
+      <c r="G13" s="1">
         <v>-31625</v>
       </c>
-      <c r="F13" s="1">
+      <c r="H13" s="1">
         <v>-33283</v>
       </c>
-      <c r="G13" s="1">
+      <c r="I13" s="1">
         <v>114</v>
       </c>
-      <c r="H13" s="1">
+      <c r="J13" s="1">
         <v>89</v>
       </c>
-      <c r="I13" s="1">
+      <c r="K13" s="1">
         <v>0.79200000000000004</v>
       </c>
-      <c r="J13" s="1">
+      <c r="L13" s="1">
         <v>1.585</v>
       </c>
-      <c r="K13" s="1">
+      <c r="M13" s="1">
         <v>0.15</v>
       </c>
-      <c r="L13" s="1">
+      <c r="N13" s="1">
         <v>0.25900000000000001</v>
       </c>
-      <c r="M13" s="3">
+      <c r="O13" s="3">
         <v>0.749</v>
       </c>
-      <c r="N13" s="2">
+      <c r="P13" s="2">
         <v>0.04</v>
       </c>
-      <c r="O13" s="2">
+      <c r="Q13" s="2">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="P13" s="2">
+      <c r="R13" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="1">
+      <c r="E14" s="1">
         <v>10117</v>
       </c>
-      <c r="D14" s="1">
+      <c r="F14" s="1">
         <v>15362</v>
       </c>
-      <c r="E14" s="1">
+      <c r="G14" s="1">
         <v>-31310</v>
       </c>
-      <c r="F14" s="1">
+      <c r="H14" s="1">
         <v>-33262</v>
       </c>
-      <c r="G14" s="1">
+      <c r="I14" s="1">
         <v>114</v>
       </c>
-      <c r="H14" s="1">
+      <c r="J14" s="1">
         <v>102</v>
       </c>
-      <c r="I14" s="1">
+      <c r="K14" s="1">
         <v>0.79700000000000004</v>
       </c>
-      <c r="J14" s="1">
+      <c r="L14" s="1">
         <v>1.591</v>
       </c>
-      <c r="K14" s="1">
+      <c r="M14" s="1">
         <v>0.14799999999999999</v>
       </c>
-      <c r="L14" s="1">
+      <c r="N14" s="1">
         <v>0.26200000000000001</v>
       </c>
-      <c r="M14" s="3">
+      <c r="O14" s="3">
         <v>0.751</v>
       </c>
-      <c r="N14" s="2">
+      <c r="P14" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="O14" s="2">
+      <c r="Q14" s="2">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="P14" s="2">
+      <c r="R14" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="1">
+      <c r="E15" s="1">
         <v>11038</v>
       </c>
-      <c r="D15" s="1">
+      <c r="F15" s="1">
         <v>13388</v>
       </c>
-      <c r="E15" s="1">
+      <c r="G15" s="1">
         <v>-30838</v>
       </c>
-      <c r="F15" s="1">
+      <c r="H15" s="1">
         <v>-33012</v>
       </c>
-      <c r="G15" s="1">
+      <c r="I15" s="1">
         <v>117</v>
       </c>
-      <c r="H15" s="1">
+      <c r="J15" s="1">
         <v>107</v>
       </c>
-      <c r="I15" s="1">
+      <c r="K15" s="1">
         <v>0.80200000000000005</v>
       </c>
-      <c r="J15" s="1">
+      <c r="L15" s="1">
         <v>1.579</v>
       </c>
-      <c r="K15" s="1">
+      <c r="M15" s="1">
         <v>0.14899999999999999</v>
       </c>
-      <c r="L15" s="1">
+      <c r="N15" s="1">
         <v>0.26400000000000001</v>
       </c>
-      <c r="M15" s="3">
+      <c r="O15" s="3">
         <v>0.747</v>
       </c>
-      <c r="N15" s="2">
+      <c r="P15" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="O15" s="2">
+      <c r="Q15" s="2">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="P15" s="2">
+      <c r="R15" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="1">
+      <c r="E16" s="1">
         <v>13212</v>
       </c>
-      <c r="D16" s="1">
+      <c r="F16" s="1">
         <v>12627</v>
       </c>
-      <c r="E16" s="1">
+      <c r="G16" s="1">
         <v>-30862</v>
       </c>
-      <c r="F16" s="1">
+      <c r="H16" s="1">
         <v>-32709</v>
       </c>
-      <c r="G16" s="1">
+      <c r="I16" s="1">
         <v>115</v>
       </c>
-      <c r="H16" s="1">
+      <c r="J16" s="1">
         <v>106</v>
       </c>
-      <c r="I16" s="1">
+      <c r="K16" s="1">
         <v>0.83099999999999996</v>
       </c>
-      <c r="J16" s="1">
+      <c r="L16" s="1">
         <v>1.575</v>
       </c>
-      <c r="K16" s="1">
+      <c r="M16" s="1">
         <v>0.151</v>
       </c>
-      <c r="L16" s="1">
+      <c r="N16" s="1">
         <v>0.26700000000000002</v>
       </c>
-      <c r="M16" s="3">
+      <c r="O16" s="3">
         <v>0.73499999999999999</v>
       </c>
-      <c r="N16" s="2">
+      <c r="P16" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="O16" s="2">
+      <c r="Q16" s="2">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="P16" s="2">
+      <c r="R16" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="1" t="s">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
issues with tidyverse and shiny packages. Needed renv::rebuild both and restart mult times. This fixed the code to add the X_Fe_OPX/CPX to the block of code and out of it's separate chunk. Trying to add dynamic axis names. Need to change the point numbers to actual number values in stead of 3/1 to avoid R not running smooth all over it and not getting lm().
</commit_message>
<xml_diff>
--- a/samp_data-prototypeT.xlsx
+++ b/samp_data-prototypeT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/17e227d69cbbef2f/Desktop/KBH_2_Pyx_Therm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{3546B046-AFE3-4B87-92BE-772B5242DA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{910D2975-E9E4-4C85-8057-2AA6CBE9DC54}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{3546B046-AFE3-4B87-92BE-772B5242DA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40DFDD72-27A5-4CB7-9FB9-1857DB43D5BE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,15 +1040,15 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
     <col min="5" max="10" width="9.140625" style="1"/>
     <col min="11" max="13" width="17.140625" style="1" customWidth="1"/>
     <col min="14" max="14" width="22.140625" style="1" customWidth="1"/>
@@ -1061,16 +1061,16 @@
   <sheetData>
     <row r="1" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1116,17 +1116,17 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E2" s="1">
         <v>-5190</v>
@@ -1172,17 +1172,17 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>-4530</v>
@@ -1228,17 +1228,17 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>1160</v>
@@ -1284,17 +1284,17 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>1247</v>
@@ -1340,17 +1340,17 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="E6" s="1">
         <v>-226</v>
@@ -1396,17 +1396,17 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="E7" s="1">
         <v>4855</v>
@@ -1452,17 +1452,17 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E8" s="1">
         <v>6610</v>
@@ -1508,17 +1508,17 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E9" s="1">
         <v>5642</v>
@@ -1564,17 +1564,17 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E10" s="1">
         <v>5332</v>
@@ -1620,17 +1620,17 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="E11" s="1">
         <v>8553</v>
@@ -1676,17 +1676,17 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="E12" s="1">
         <v>8960</v>
@@ -1732,17 +1732,17 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E13" s="1">
         <v>9599</v>
@@ -1788,17 +1788,17 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E14" s="1">
         <v>10117</v>
@@ -1844,17 +1844,17 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E15" s="1">
         <v>11038</v>
@@ -1900,17 +1900,17 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E16" s="1">
         <v>13212</v>

</xml_diff>

<commit_message>
fixed issues with the n/a at teh bottom of the charts added download csv file button deployed to take over the world
</commit_message>
<xml_diff>
--- a/samp_data-prototypeT.xlsx
+++ b/samp_data-prototypeT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/17e227d69cbbef2f/Desktop/KBH_2_Pyx_Therm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{3546B046-AFE3-4B87-92BE-772B5242DA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40DFDD72-27A5-4CB7-9FB9-1857DB43D5BE}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{3546B046-AFE3-4B87-92BE-772B5242DA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{895964FD-D03C-49AE-A6A9-834F613D00AF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
   <si>
     <t>rim</t>
   </si>
@@ -41,27 +41,6 @@
   </si>
   <si>
     <t>core</t>
-  </si>
-  <si>
-    <t>X_CPX</t>
-  </si>
-  <si>
-    <t>X_OPX</t>
-  </si>
-  <si>
-    <t>Y_CPX</t>
-  </si>
-  <si>
-    <t>Y_OPX</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Z_CPX</t>
-  </si>
-  <si>
-    <t>Z_OPX</t>
   </si>
   <si>
     <t>Nb_ions_Mg_CPX</t>
@@ -98,96 +77,6 @@
   </si>
   <si>
     <t>point_number_OPX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 1 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 2 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 3 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 4 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 5 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 6 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 7 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 8 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 9 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 10 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 11 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 12 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 13 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 14 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 / 15 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 1 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 2 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 3 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 4 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 5 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 6 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 7 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 8 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 9 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 10 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 11 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 12 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 13 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 14 . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 / 15 . </t>
   </si>
 </sst>
 </file>
@@ -1037,11 +926,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1049,28 +936,27 @@
     <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
-    <col min="5" max="10" width="9.140625" style="1"/>
-    <col min="11" max="13" width="17.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="7" width="17.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1085,879 +971,586 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>-5190</v>
+        <v>0.84599999999999997</v>
       </c>
       <c r="F2" s="1">
-        <v>-5855</v>
+        <v>1.6379999999999999</v>
       </c>
       <c r="G2" s="1">
-        <v>-27104</v>
+        <v>0.128</v>
       </c>
       <c r="H2" s="1">
-        <v>-24690</v>
-      </c>
-      <c r="I2" s="1">
-        <v>139</v>
-      </c>
-      <c r="J2" s="1">
-        <v>150</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0.84599999999999997</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1.6379999999999999</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0.128</v>
-      </c>
-      <c r="N2" s="1">
         <v>0.222</v>
       </c>
-      <c r="O2" s="3">
+      <c r="I2" s="3">
         <v>0.74299999999999999</v>
       </c>
-      <c r="P2" s="2">
+      <c r="J2" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="K2" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="R2" s="2">
+      <c r="L2" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>24</v>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>-4530</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="F3" s="1">
-        <v>-5032</v>
+        <v>1.62</v>
       </c>
       <c r="G3" s="1">
-        <v>-27162</v>
+        <v>0.127</v>
       </c>
       <c r="H3" s="1">
-        <v>-25438</v>
-      </c>
-      <c r="I3" s="1">
-        <v>139</v>
-      </c>
-      <c r="J3" s="1">
-        <v>146</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1.62</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0.127</v>
-      </c>
-      <c r="N3" s="1">
         <v>0.22600000000000001</v>
       </c>
-      <c r="O3" s="3">
+      <c r="I3" s="3">
         <v>0.74099999999999999</v>
       </c>
-      <c r="P3" s="2">
+      <c r="J3" s="2">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="K3" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="R3" s="2">
+      <c r="L3" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
       </c>
       <c r="E4" s="1">
-        <v>1160</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="F4" s="1">
-        <v>-3176</v>
+        <v>1.6359999999999999</v>
       </c>
       <c r="G4" s="1">
-        <v>-29155</v>
+        <v>0.127</v>
       </c>
       <c r="H4" s="1">
-        <v>-27901</v>
-      </c>
-      <c r="I4" s="1">
-        <v>129</v>
-      </c>
-      <c r="J4" s="1">
-        <v>138</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0.84499999999999997</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1.6359999999999999</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0.127</v>
-      </c>
-      <c r="N4" s="1">
         <v>0.22500000000000001</v>
       </c>
-      <c r="O4" s="3">
+      <c r="I4" s="3">
         <v>0.73699999999999999</v>
       </c>
-      <c r="P4" s="2">
+      <c r="J4" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="K4" s="2">
         <v>0.10100000000000001</v>
       </c>
-      <c r="R4" s="2">
+      <c r="L4" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>26</v>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
       </c>
       <c r="E5" s="1">
-        <v>1247</v>
+        <v>0.84</v>
       </c>
       <c r="F5" s="1">
-        <v>162</v>
+        <v>1.623</v>
       </c>
       <c r="G5" s="1">
-        <v>-30822</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="H5" s="1">
-        <v>-28862</v>
-      </c>
-      <c r="I5" s="1">
-        <v>128</v>
-      </c>
-      <c r="J5" s="1">
-        <v>135</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1.623</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="N5" s="1">
         <v>0.23100000000000001</v>
       </c>
-      <c r="O5" s="3">
+      <c r="I5" s="3">
         <v>0.746</v>
       </c>
-      <c r="P5" s="2">
+      <c r="J5" s="2">
         <v>3.9E-2</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="K5" s="2">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="R5" s="2">
+      <c r="L5" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>27</v>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5</v>
       </c>
       <c r="E6" s="1">
-        <v>-226</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="F6" s="1">
-        <v>2688</v>
+        <v>1.5960000000000001</v>
       </c>
       <c r="G6" s="1">
-        <v>-31114</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="H6" s="1">
-        <v>-29738</v>
-      </c>
-      <c r="I6" s="1">
-        <v>124</v>
-      </c>
-      <c r="J6" s="1">
-        <v>127</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0.84499999999999997</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1.5960000000000001</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="N6" s="1">
         <v>0.249</v>
       </c>
-      <c r="O6" s="3">
+      <c r="I6" s="3">
         <v>0.74</v>
       </c>
-      <c r="P6" s="2">
+      <c r="J6" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="K6" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="R6" s="2">
+      <c r="L6" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>28</v>
+      <c r="C7" s="3">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3">
+        <v>6</v>
       </c>
       <c r="E7" s="1">
-        <v>4855</v>
+        <v>0.83</v>
       </c>
       <c r="F7" s="1">
-        <v>3403</v>
+        <v>1.593</v>
       </c>
       <c r="G7" s="1">
-        <v>-31987</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="H7" s="1">
-        <v>-26027</v>
-      </c>
-      <c r="I7" s="1">
-        <v>117</v>
-      </c>
-      <c r="J7" s="1">
-        <v>140</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1.593</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="N7" s="1">
         <v>0.249</v>
       </c>
-      <c r="O7" s="3">
+      <c r="I7" s="3">
         <v>0.74</v>
       </c>
-      <c r="P7" s="2">
+      <c r="J7" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="K7" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="R7" s="2">
+      <c r="L7" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>29</v>
+      <c r="C8" s="3">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
+        <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>6610</v>
+        <v>0.81200000000000006</v>
       </c>
       <c r="F8" s="1">
-        <v>11338</v>
+        <v>1.5860000000000001</v>
       </c>
       <c r="G8" s="1">
-        <v>-32138</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="H8" s="1">
-        <v>-28588</v>
-      </c>
-      <c r="I8" s="1">
-        <v>117</v>
-      </c>
-      <c r="J8" s="1">
-        <v>120</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0.81200000000000006</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1.5860000000000001</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="N8" s="1">
         <v>0.25700000000000001</v>
       </c>
-      <c r="O8" s="3">
+      <c r="I8" s="3">
         <v>0.751</v>
       </c>
-      <c r="P8" s="2">
+      <c r="J8" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="K8" s="2">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="R8" s="2">
+      <c r="L8" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>30</v>
+      <c r="C9" s="3">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>8</v>
       </c>
       <c r="E9" s="1">
-        <v>5642</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="F9" s="1">
-        <v>12212</v>
+        <v>1.5920000000000001</v>
       </c>
       <c r="G9" s="1">
-        <v>-31195</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="H9" s="1">
-        <v>-27364</v>
-      </c>
-      <c r="I9" s="1">
-        <v>123</v>
-      </c>
-      <c r="J9" s="1">
-        <v>124</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="L9" s="1">
-        <v>1.5920000000000001</v>
-      </c>
-      <c r="M9" s="1">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="N9" s="1">
         <v>0.25800000000000001</v>
       </c>
-      <c r="O9" s="3">
+      <c r="I9" s="3">
         <v>0.748</v>
       </c>
-      <c r="P9" s="2">
+      <c r="J9" s="2">
         <v>3.9E-2</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="K9" s="2">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="R9" s="2">
+      <c r="L9" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>31</v>
+      <c r="C10" s="3">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3">
+        <v>9</v>
       </c>
       <c r="E10" s="1">
-        <v>5332</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="F10" s="1">
-        <v>12355</v>
+        <v>1.6</v>
       </c>
       <c r="G10" s="1">
-        <v>-31292</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="H10" s="1">
-        <v>-24835</v>
-      </c>
-      <c r="I10" s="1">
-        <v>123</v>
-      </c>
-      <c r="J10" s="1">
-        <v>133</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="L10" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="M10" s="1">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="N10" s="1">
         <v>0.255</v>
       </c>
-      <c r="O10" s="3">
+      <c r="I10" s="3">
         <v>0.82099999999999995</v>
       </c>
-      <c r="P10" s="2">
+      <c r="J10" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="K10" s="2">
         <v>4.7E-2</v>
       </c>
-      <c r="R10" s="2">
+      <c r="L10" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>32</v>
+      <c r="C11" s="3">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3">
+        <v>10</v>
       </c>
       <c r="E11" s="1">
-        <v>8553</v>
+        <v>0.78900000000000003</v>
       </c>
       <c r="F11" s="1">
-        <v>13901</v>
+        <v>1.601</v>
       </c>
       <c r="G11" s="1">
-        <v>-33012</v>
+        <v>0.151</v>
       </c>
       <c r="H11" s="1">
-        <v>-24749</v>
-      </c>
-      <c r="I11" s="1">
-        <v>108</v>
-      </c>
-      <c r="J11" s="1">
-        <v>124</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0.78900000000000003</v>
-      </c>
-      <c r="L11" s="1">
-        <v>1.601</v>
-      </c>
-      <c r="M11" s="1">
-        <v>0.151</v>
-      </c>
-      <c r="N11" s="1">
         <v>0.24399999999999999</v>
       </c>
-      <c r="O11" s="3">
+      <c r="I11" s="3">
         <v>0.752</v>
       </c>
-      <c r="P11" s="2">
+      <c r="J11" s="2">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="K11" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="R11" s="2">
+      <c r="L11" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>33</v>
+      <c r="C12" s="3">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3">
+        <v>11</v>
       </c>
       <c r="E12" s="1">
-        <v>8960</v>
+        <v>0.88700000000000001</v>
       </c>
       <c r="F12" s="1">
-        <v>17511</v>
+        <v>1.5880000000000001</v>
       </c>
       <c r="G12" s="1">
-        <v>-32963</v>
+        <v>0.108</v>
       </c>
       <c r="H12" s="1">
-        <v>-25622</v>
-      </c>
-      <c r="I12" s="1">
-        <v>108</v>
-      </c>
-      <c r="J12" s="1">
-        <v>116</v>
-      </c>
-      <c r="K12" s="1">
-        <v>0.88700000000000001</v>
-      </c>
-      <c r="L12" s="1">
-        <v>1.5880000000000001</v>
-      </c>
-      <c r="M12" s="1">
-        <v>0.108</v>
-      </c>
-      <c r="N12" s="1">
         <v>0.26400000000000001</v>
       </c>
-      <c r="O12" s="3">
+      <c r="I12" s="3">
         <v>0.83</v>
       </c>
-      <c r="P12" s="2">
+      <c r="J12" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="K12" s="2">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="R12" s="2">
+      <c r="L12" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>34</v>
+      <c r="C13" s="3">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3">
+        <v>12</v>
       </c>
       <c r="E13" s="1">
-        <v>9599</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="F13" s="1">
-        <v>18357</v>
+        <v>1.585</v>
       </c>
       <c r="G13" s="1">
-        <v>-31625</v>
+        <v>0.15</v>
       </c>
       <c r="H13" s="1">
-        <v>-33283</v>
-      </c>
-      <c r="I13" s="1">
-        <v>114</v>
-      </c>
-      <c r="J13" s="1">
-        <v>89</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0.79200000000000004</v>
-      </c>
-      <c r="L13" s="1">
-        <v>1.585</v>
-      </c>
-      <c r="M13" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="N13" s="1">
         <v>0.25900000000000001</v>
       </c>
-      <c r="O13" s="3">
+      <c r="I13" s="3">
         <v>0.749</v>
       </c>
-      <c r="P13" s="2">
+      <c r="J13" s="2">
         <v>0.04</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="K13" s="2">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="R13" s="2">
+      <c r="L13" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>35</v>
+      <c r="C14" s="3">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3">
+        <v>13</v>
       </c>
       <c r="E14" s="1">
-        <v>10117</v>
+        <v>0.79700000000000004</v>
       </c>
       <c r="F14" s="1">
-        <v>15362</v>
+        <v>1.591</v>
       </c>
       <c r="G14" s="1">
-        <v>-31310</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="H14" s="1">
-        <v>-33262</v>
-      </c>
-      <c r="I14" s="1">
-        <v>114</v>
-      </c>
-      <c r="J14" s="1">
-        <v>102</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0.79700000000000004</v>
-      </c>
-      <c r="L14" s="1">
-        <v>1.591</v>
-      </c>
-      <c r="M14" s="1">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="N14" s="1">
         <v>0.26200000000000001</v>
       </c>
-      <c r="O14" s="3">
+      <c r="I14" s="3">
         <v>0.751</v>
       </c>
-      <c r="P14" s="2">
+      <c r="J14" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="K14" s="2">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="R14" s="2">
+      <c r="L14" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>36</v>
+      <c r="C15" s="3">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3">
+        <v>14</v>
       </c>
       <c r="E15" s="1">
-        <v>11038</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="F15" s="1">
-        <v>13388</v>
+        <v>1.579</v>
       </c>
       <c r="G15" s="1">
-        <v>-30838</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="H15" s="1">
-        <v>-33012</v>
-      </c>
-      <c r="I15" s="1">
-        <v>117</v>
-      </c>
-      <c r="J15" s="1">
-        <v>107</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0.80200000000000005</v>
-      </c>
-      <c r="L15" s="1">
-        <v>1.579</v>
-      </c>
-      <c r="M15" s="1">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="N15" s="1">
         <v>0.26400000000000001</v>
       </c>
-      <c r="O15" s="3">
+      <c r="I15" s="3">
         <v>0.747</v>
       </c>
-      <c r="P15" s="2">
+      <c r="J15" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="K15" s="2">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="R15" s="2">
+      <c r="L15" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>37</v>
+      <c r="C16" s="3">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3">
+        <v>15</v>
       </c>
       <c r="E16" s="1">
-        <v>13212</v>
+        <v>0.83099999999999996</v>
       </c>
       <c r="F16" s="1">
-        <v>12627</v>
+        <v>1.575</v>
       </c>
       <c r="G16" s="1">
-        <v>-30862</v>
+        <v>0.151</v>
       </c>
       <c r="H16" s="1">
-        <v>-32709</v>
-      </c>
-      <c r="I16" s="1">
-        <v>115</v>
-      </c>
-      <c r="J16" s="1">
-        <v>106</v>
-      </c>
-      <c r="K16" s="1">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="L16" s="1">
-        <v>1.575</v>
-      </c>
-      <c r="M16" s="1">
-        <v>0.151</v>
-      </c>
-      <c r="N16" s="1">
         <v>0.26700000000000002</v>
       </c>
-      <c r="O16" s="3">
+      <c r="I16" s="3">
         <v>0.73499999999999999</v>
       </c>
-      <c r="P16" s="2">
+      <c r="J16" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="K16" s="2">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="R16" s="2">
+      <c r="L16" s="2">
         <v>8.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>